<commit_message>
update final project web
</commit_message>
<xml_diff>
--- a/Final Project Web/Final Project Web Test Scenario - Mikail Gibran Fernanda Lubis.xlsx
+++ b/Final Project Web/Final Project Web Test Scenario - Mikail Gibran Fernanda Lubis.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\095097\Katalon Studio\Final Project - Web UI - Katakoki\Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\095097\Katalon Studio\Final Project - Web UI - Katakoki\Final Project Web\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,12 +15,11 @@
     <sheet name="User" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="81">
   <si>
     <t>Created By</t>
   </si>
@@ -255,6 +254,21 @@
   <si>
     <t>TC_006</t>
   </si>
+  <si>
+    <t>Add to Cart</t>
+  </si>
+  <si>
+    <t>5. verify product added</t>
+  </si>
+  <si>
+    <t>product added</t>
+  </si>
+  <si>
+    <t>passed</t>
+  </si>
+  <si>
+    <t>TC_007</t>
+  </si>
 </sst>
 </file>
 
@@ -313,7 +327,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -423,77 +437,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -507,51 +450,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -593,109 +496,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -715,26 +531,30 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -951,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC993"/>
+  <dimension ref="A1:AC992"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -977,23 +797,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57"/>
+      <c r="B1" s="24"/>
       <c r="C1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="56" t="s">
+      <c r="F1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="57"/>
-      <c r="H1" s="58" t="s">
+      <c r="G1" s="24"/>
+      <c r="H1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="59"/>
+      <c r="I1" s="26"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -1047,23 +867,23 @@
       <c r="AC2" s="3"/>
     </row>
     <row r="3" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="57"/>
+      <c r="B3" s="24"/>
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="61" t="s">
+      <c r="F3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="57"/>
-      <c r="H3" s="62">
+      <c r="G3" s="24"/>
+      <c r="H3" s="29">
         <v>44742</v>
       </c>
-      <c r="I3" s="59"/>
+      <c r="I3" s="26"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
@@ -1117,16 +937,16 @@
       <c r="AC4" s="3"/>
     </row>
     <row r="5" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="61" t="s">
+      <c r="A5" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="57"/>
+      <c r="B5" s="24"/>
       <c r="C5" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="46" t="s">
+      <c r="F5" s="30" t="s">
         <v>7</v>
       </c>
       <c r="G5" s="9" t="s">
@@ -1165,7 +985,7 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="47"/>
+      <c r="F6" s="31"/>
       <c r="G6" s="12">
         <v>1</v>
       </c>
@@ -1228,32 +1048,32 @@
       <c r="AC7" s="3"/>
     </row>
     <row r="8" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="48" t="s">
+      <c r="E8" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="49"/>
-      <c r="G8" s="18" t="s">
+      <c r="F8" s="20"/>
+      <c r="G8" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="36" t="s">
         <v>18</v>
       </c>
       <c r="K8" s="3"/>
@@ -1277,30 +1097,30 @@
       <c r="AC8" s="3"/>
     </row>
     <row r="9" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="50" t="s">
+      <c r="A9" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="65" t="s">
+      <c r="C9" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="D9" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="53" t="s">
+      <c r="E9" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="54"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="3" t="s">
+      <c r="F9" s="21"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="I9" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="22"/>
+      <c r="J9" s="16"/>
       <c r="K9" s="3"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
@@ -1322,22 +1142,22 @@
       <c r="AC9" s="3"/>
     </row>
     <row r="10" spans="1:29" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="51"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="66"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="53" t="s">
+      <c r="A10" s="20"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="54"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="23" t="s">
+      <c r="F10" s="21"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="20" t="s">
+      <c r="I10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="22"/>
+      <c r="J10" s="16"/>
       <c r="K10" s="3"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
@@ -1359,20 +1179,20 @@
       <c r="AC10" s="3"/>
     </row>
     <row r="11" spans="1:29" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="51"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="66"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="53" t="s">
+      <c r="A11" s="20"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="54"/>
-      <c r="G11" s="20" t="s">
+      <c r="F11" s="21"/>
+      <c r="G11" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="23"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="22"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
       <c r="K11" s="3"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
@@ -1394,22 +1214,22 @@
       <c r="AC11" s="3"/>
     </row>
     <row r="12" spans="1:29" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="52"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="67"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="63" t="s">
+      <c r="A12" s="20"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="64"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="25" t="s">
+      <c r="F12" s="20"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="I12" s="24" t="s">
+      <c r="I12" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="J12" s="26" t="s">
+      <c r="J12" s="16" t="s">
         <v>9</v>
       </c>
       <c r="K12" s="3"/>
@@ -1433,28 +1253,28 @@
       <c r="AC12" s="3"/>
     </row>
     <row r="13" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="65" t="s">
+      <c r="B13" s="32"/>
+      <c r="C13" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="53" t="s">
+      <c r="E13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="54"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="3" t="s">
+      <c r="F13" s="21"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="21" t="s">
+      <c r="I13" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="J13" s="22"/>
+      <c r="J13" s="16"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
@@ -1476,22 +1296,22 @@
       <c r="AC13" s="3"/>
     </row>
     <row r="14" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="51"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="66"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="53" t="s">
+      <c r="A14" s="20"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="54"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="23" t="s">
+      <c r="F14" s="21"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="I14" s="20" t="s">
+      <c r="I14" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="J14" s="22"/>
+      <c r="J14" s="16"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
@@ -1513,20 +1333,20 @@
       <c r="AC14" s="3"/>
     </row>
     <row r="15" spans="1:29" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="51"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="66"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="53" t="s">
+      <c r="A15" s="20"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="F15" s="54"/>
-      <c r="G15" s="20" t="s">
+      <c r="F15" s="21"/>
+      <c r="G15" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="23"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="22"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
@@ -1548,22 +1368,22 @@
       <c r="AC15" s="3"/>
     </row>
     <row r="16" spans="1:29" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="51"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="66"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="44" t="s">
+      <c r="A16" s="20"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="45"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="23" t="s">
+      <c r="F16" s="20"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="I16" s="20" t="s">
+      <c r="I16" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="J16" s="27" t="s">
+      <c r="J16" s="38" t="s">
         <v>8</v>
       </c>
       <c r="K16" s="5"/>
@@ -1587,30 +1407,30 @@
       <c r="AC16" s="3"/>
     </row>
     <row r="17" spans="1:29" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="70" t="s">
+      <c r="B17" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="D17" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="35" t="s">
+      <c r="E17" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="42"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="31" t="s">
+      <c r="F17" s="21"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="I17" s="32" t="s">
+      <c r="I17" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="J17" s="28"/>
+      <c r="J17" s="15"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
@@ -1632,24 +1452,24 @@
       <c r="AC17" s="3"/>
     </row>
     <row r="18" spans="1:29" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="34"/>
-      <c r="B18" s="71"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="35" t="s">
+      <c r="A18" s="18"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="42"/>
-      <c r="G18" s="31" t="s">
+      <c r="F18" s="21"/>
+      <c r="G18" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="32" t="s">
+      <c r="H18" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="I18" s="32" t="s">
+      <c r="I18" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="29"/>
+      <c r="J18" s="15"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
@@ -1671,20 +1491,20 @@
       <c r="AC18" s="3"/>
     </row>
     <row r="19" spans="1:29" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="34"/>
-      <c r="B19" s="71"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="35" t="s">
+      <c r="A19" s="18"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="F19" s="43"/>
-      <c r="G19" s="32" t="s">
+      <c r="F19" s="33"/>
+      <c r="G19" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="29"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
@@ -1706,20 +1526,20 @@
       <c r="AC19" s="3"/>
     </row>
     <row r="20" spans="1:29" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="34"/>
-      <c r="B20" s="71"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="35" t="s">
+      <c r="A20" s="18"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F20" s="36"/>
-      <c r="G20" s="31" t="s">
+      <c r="F20" s="20"/>
+      <c r="G20" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="29"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
@@ -1741,22 +1561,22 @@
       <c r="AC20" s="3"/>
     </row>
     <row r="21" spans="1:29" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="34"/>
-      <c r="B21" s="71"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="35" t="s">
+      <c r="A21" s="18"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="F21" s="36"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="31" t="s">
+      <c r="F21" s="20"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="I21" s="31" t="s">
+      <c r="I21" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="J21" s="30" t="s">
+      <c r="J21" s="15" t="s">
         <v>8</v>
       </c>
       <c r="K21" s="3"/>
@@ -1780,26 +1600,26 @@
       <c r="AC21" s="3"/>
     </row>
     <row r="22" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="71"/>
-      <c r="C22" s="41" t="s">
+      <c r="B22" s="32"/>
+      <c r="C22" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="35" t="s">
+      <c r="E22" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="42"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="31" t="s">
+      <c r="F22" s="21"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="I22" s="32"/>
-      <c r="J22" s="28"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
@@ -1821,20 +1641,20 @@
       <c r="AC22" s="3"/>
     </row>
     <row r="23" spans="1:29" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="34"/>
-      <c r="B23" s="71"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="35" t="s">
+      <c r="A23" s="18"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="42"/>
-      <c r="G23" s="31" t="s">
+      <c r="F23" s="21"/>
+      <c r="G23" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="29"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
@@ -1856,20 +1676,20 @@
       <c r="AC23" s="3"/>
     </row>
     <row r="24" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="34"/>
-      <c r="B24" s="71"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="35" t="s">
+      <c r="A24" s="18"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="F24" s="42"/>
-      <c r="G24" s="32" t="s">
+      <c r="F24" s="21"/>
+      <c r="G24" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="29"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
@@ -1891,19 +1711,20 @@
       <c r="AC24" s="3"/>
     </row>
     <row r="25" spans="1:29" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="34"/>
-      <c r="B25" s="71"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="35" t="s">
+      <c r="A25" s="18"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F25" s="36"/>
-      <c r="G25" s="31" t="s">
+      <c r="F25" s="20"/>
+      <c r="G25" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
@@ -1925,22 +1746,22 @@
       <c r="AC25" s="3"/>
     </row>
     <row r="26" spans="1:29" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="34"/>
-      <c r="B26" s="71"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="35" t="s">
+      <c r="A26" s="18"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="F26" s="36"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="31" t="s">
+      <c r="F26" s="20"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="I26" s="31" t="s">
+      <c r="I26" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="J26" s="30" t="s">
+      <c r="J26" s="15" t="s">
         <v>9</v>
       </c>
       <c r="K26" s="3"/>
@@ -1964,28 +1785,28 @@
       <c r="AC26" s="3"/>
     </row>
     <row r="27" spans="1:29" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="71"/>
-      <c r="C27" s="34" t="s">
+      <c r="B27" s="32"/>
+      <c r="C27" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="D27" s="34" t="s">
+      <c r="D27" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="35" t="s">
+      <c r="E27" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F27" s="36"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="32" t="s">
+      <c r="F27" s="20"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="I27" s="32" t="s">
+      <c r="I27" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="J27" s="32"/>
+      <c r="J27" s="15"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
@@ -2007,22 +1828,22 @@
       <c r="AC27" s="3"/>
     </row>
     <row r="28" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="34"/>
-      <c r="B28" s="71"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="35" t="s">
+      <c r="A28" s="18"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="36"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32" t="s">
+      <c r="F28" s="20"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="I28" s="32" t="s">
+      <c r="I28" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="J28" s="32"/>
+      <c r="J28" s="15"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
@@ -2044,22 +1865,22 @@
       <c r="AC28" s="3"/>
     </row>
     <row r="29" spans="1:29" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="34"/>
-      <c r="B29" s="71"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="35" t="s">
+      <c r="A29" s="18"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="F29" s="36"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32" t="s">
+      <c r="F29" s="20"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="I29" s="32" t="s">
+      <c r="I29" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="J29" s="32"/>
+      <c r="J29" s="15"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
@@ -2081,22 +1902,22 @@
       <c r="AC29" s="3"/>
     </row>
     <row r="30" spans="1:29" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="34"/>
-      <c r="B30" s="71"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="35" t="s">
+      <c r="A30" s="18"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="F30" s="36"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="32" t="s">
+      <c r="F30" s="20"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="I30" s="32" t="s">
+      <c r="I30" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="J30" s="32"/>
+      <c r="J30" s="15"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
@@ -2118,20 +1939,20 @@
       <c r="AC30" s="3"/>
     </row>
     <row r="31" spans="1:29" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="34"/>
-      <c r="B31" s="71"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="35" t="s">
+      <c r="A31" s="18"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="36"/>
-      <c r="G31" s="32" t="s">
+      <c r="F31" s="20"/>
+      <c r="G31" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="32"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
@@ -2153,22 +1974,22 @@
       <c r="AC31" s="3"/>
     </row>
     <row r="32" spans="1:29" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="34"/>
-      <c r="B32" s="71"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="35" t="s">
+      <c r="A32" s="18"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="F32" s="36"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="32" t="s">
+      <c r="F32" s="20"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="I32" s="32" t="s">
+      <c r="I32" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="J32" s="32" t="s">
+      <c r="J32" s="15" t="s">
         <v>8</v>
       </c>
       <c r="K32" s="3"/>
@@ -2192,28 +2013,28 @@
       <c r="AC32" s="3"/>
     </row>
     <row r="33" spans="1:29" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="68" t="s">
+      <c r="A33" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="71"/>
-      <c r="C33" s="34" t="s">
+      <c r="B33" s="32"/>
+      <c r="C33" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="D33" s="34" t="s">
+      <c r="D33" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="E33" s="35" t="s">
+      <c r="E33" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F33" s="36"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32" t="s">
+      <c r="F33" s="20"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="I33" s="32" t="s">
+      <c r="I33" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="J33" s="32"/>
+      <c r="J33" s="15"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -2235,22 +2056,22 @@
       <c r="AC33" s="3"/>
     </row>
     <row r="34" spans="1:29" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="69"/>
-      <c r="B34" s="71"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="35" t="s">
+      <c r="A34" s="18"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F34" s="36"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="32" t="s">
+      <c r="F34" s="20"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="I34" s="32" t="s">
+      <c r="I34" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="J34" s="32"/>
+      <c r="J34" s="15"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
@@ -2272,22 +2093,22 @@
       <c r="AC34" s="3"/>
     </row>
     <row r="35" spans="1:29" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="69"/>
-      <c r="B35" s="71"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="35" t="s">
+      <c r="A35" s="18"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="F35" s="36"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32" t="s">
+      <c r="F35" s="20"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="I35" s="32" t="s">
+      <c r="I35" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="J35" s="32"/>
+      <c r="J35" s="15"/>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
@@ -2309,22 +2130,22 @@
       <c r="AC35" s="3"/>
     </row>
     <row r="36" spans="1:29" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="69"/>
-      <c r="B36" s="71"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="35" t="s">
+      <c r="A36" s="18"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="F36" s="36"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32" t="s">
+      <c r="F36" s="20"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="I36" s="32" t="s">
+      <c r="I36" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="J36" s="32"/>
+      <c r="J36" s="15"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
@@ -2346,20 +2167,20 @@
       <c r="AC36" s="3"/>
     </row>
     <row r="37" spans="1:29" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="69"/>
-      <c r="B37" s="71"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="35" t="s">
+      <c r="A37" s="18"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="F37" s="36"/>
-      <c r="G37" s="32" t="s">
+      <c r="F37" s="20"/>
+      <c r="G37" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="H37" s="32"/>
-      <c r="I37" s="32"/>
-      <c r="J37" s="32"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
@@ -2381,22 +2202,22 @@
       <c r="AC37" s="3"/>
     </row>
     <row r="38" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="69"/>
-      <c r="B38" s="71"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="35" t="s">
+      <c r="A38" s="18"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="F38" s="36"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="32" t="s">
+      <c r="F38" s="20"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="I38" s="32" t="s">
+      <c r="I38" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="J38" s="32" t="s">
+      <c r="J38" s="15" t="s">
         <v>8</v>
       </c>
       <c r="K38" s="3"/>
@@ -2420,26 +2241,28 @@
       <c r="AC38" s="3"/>
     </row>
     <row r="39" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="D39" s="34" t="s">
+      <c r="A39" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" s="32"/>
+      <c r="C39" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="E39" s="35" t="s">
+      <c r="E39" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F39" s="36"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="32" t="s">
+      <c r="F39" s="20"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="I39" s="32" t="s">
+      <c r="I39" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="J39" s="32"/>
+      <c r="J39" s="15"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
@@ -2460,23 +2283,23 @@
       <c r="AB39" s="3"/>
       <c r="AC39" s="3"/>
     </row>
-    <row r="40" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="35" t="s">
+    <row r="40" spans="1:29" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="18"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F40" s="36"/>
-      <c r="G40" s="32"/>
-      <c r="H40" s="32" t="s">
+      <c r="F40" s="20"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="I40" s="32" t="s">
+      <c r="I40" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="J40" s="32"/>
+      <c r="J40" s="15"/>
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
@@ -2497,23 +2320,23 @@
       <c r="AB40" s="3"/>
       <c r="AC40" s="3"/>
     </row>
-    <row r="41" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="35" t="s">
+    <row r="41" spans="1:29" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="18"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="F41" s="36"/>
-      <c r="G41" s="32"/>
-      <c r="H41" s="32" t="s">
+      <c r="F41" s="20"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="I41" s="32" t="s">
+      <c r="I41" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="J41" s="32"/>
+      <c r="J41" s="15"/>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
@@ -2534,23 +2357,23 @@
       <c r="AB41" s="3"/>
       <c r="AC41" s="3"/>
     </row>
-    <row r="42" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="34"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="35" t="s">
+    <row r="42" spans="1:29" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="18"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="F42" s="36"/>
-      <c r="G42" s="32"/>
-      <c r="H42" s="32" t="s">
+      <c r="F42" s="20"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="I42" s="32" t="s">
+      <c r="I42" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="J42" s="32"/>
+      <c r="J42" s="15"/>
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
@@ -2571,21 +2394,25 @@
       <c r="AB42" s="3"/>
       <c r="AC42" s="3"/>
     </row>
-    <row r="43" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="34"/>
-      <c r="E43" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="F43" s="36"/>
-      <c r="G43" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="H43" s="32"/>
-      <c r="I43" s="32"/>
-      <c r="J43" s="32"/>
+    <row r="43" spans="1:29" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="18"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="F43" s="19"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="I43" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="J43" s="15" t="s">
+        <v>79</v>
+      </c>
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
@@ -2609,22 +2436,14 @@
     <row r="44" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="34"/>
-      <c r="E44" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="F44" s="36"/>
-      <c r="G44" s="32"/>
-      <c r="H44" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="I44" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="J44" s="32" t="s">
-        <v>8</v>
-      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
@@ -7605,7 +7424,7 @@
       <c r="AB204" s="3"/>
       <c r="AC204" s="3"/>
     </row>
-    <row r="205" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="3"/>
       <c r="B205" s="3"/>
       <c r="C205" s="3"/>
@@ -7853,37 +7672,7 @@
       <c r="AB212" s="3"/>
       <c r="AC212" s="3"/>
     </row>
-    <row r="213" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A213" s="3"/>
-      <c r="B213" s="3"/>
-      <c r="C213" s="3"/>
-      <c r="D213" s="3"/>
-      <c r="E213" s="3"/>
-      <c r="F213" s="3"/>
-      <c r="G213" s="3"/>
-      <c r="H213" s="3"/>
-      <c r="I213" s="3"/>
-      <c r="J213" s="3"/>
-      <c r="K213" s="3"/>
-      <c r="L213" s="3"/>
-      <c r="M213" s="3"/>
-      <c r="N213" s="3"/>
-      <c r="O213" s="3"/>
-      <c r="P213" s="3"/>
-      <c r="Q213" s="3"/>
-      <c r="R213" s="3"/>
-      <c r="S213" s="3"/>
-      <c r="T213" s="3"/>
-      <c r="U213" s="3"/>
-      <c r="V213" s="3"/>
-      <c r="W213" s="3"/>
-      <c r="X213" s="3"/>
-      <c r="Y213" s="3"/>
-      <c r="Z213" s="3"/>
-      <c r="AA213" s="3"/>
-      <c r="AB213" s="3"/>
-      <c r="AC213" s="3"/>
-    </row>
+    <row r="213" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="214" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="215" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="216" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8663,34 +8452,35 @@
     <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="C33:C38"/>
-    <mergeCell ref="D33:D38"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="A33:A38"/>
-    <mergeCell ref="B17:B38"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="D22:D26"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="C39:C43"/>
+    <mergeCell ref="D39:D43"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="B9:B16"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="D17:D21"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B17:B43"/>
+    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
     <mergeCell ref="C22:C26"/>
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A1:B1"/>
@@ -8707,32 +8497,30 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="E15:F15"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="B9:B16"/>
-    <mergeCell ref="D9:D12"/>
-    <mergeCell ref="D13:D16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="C17:C21"/>
-    <mergeCell ref="D17:D21"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="C39:C44"/>
-    <mergeCell ref="D39:D44"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="D22:D26"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="C33:C38"/>
+    <mergeCell ref="D33:D38"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="A33:A38"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="D27:D32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>